<commit_message>
Game class and udgrade methods with some exceptions
</commit_message>
<xml_diff>
--- a/base de datos proyectro.xlsx
+++ b/base de datos proyectro.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chuyi\OneDrive - Universidad de Guadalajara\proyecto modular\Modular\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC2F1CFD-E06D-4C59-BE29-88936E2E43BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D2760A-0E3D-41CB-9BF9-F54D7DD5229C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{E867A700-DDBB-4E62-BEA2-0A2010D09D0F}"/>
+    <workbookView xWindow="23040" yWindow="0" windowWidth="11520" windowHeight="12960" xr2:uid="{E867A700-DDBB-4E62-BEA2-0A2010D09D0F}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="57">
   <si>
     <t xml:space="preserve">String </t>
   </si>
@@ -59,12 +59,6 @@
     <t>name</t>
   </si>
   <si>
-    <t>cedula</t>
-  </si>
-  <si>
-    <t>Cadula profecional</t>
-  </si>
-  <si>
     <t>Password</t>
   </si>
   <si>
@@ -198,6 +192,21 @@
   </si>
   <si>
     <t>Juego</t>
+  </si>
+  <si>
+    <t>las name</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>int cliente</t>
   </si>
 </sst>
 </file>
@@ -245,7 +254,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -268,11 +277,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -282,6 +302,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -597,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E69598C8-3E91-45F2-9B76-B94EC4562CE2}">
-  <dimension ref="A2:G36"/>
+  <dimension ref="A2:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -655,10 +678,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C6">
         <v>121</v>
@@ -669,13 +692,13 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C7">
         <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -683,7 +706,7 @@
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C8">
         <v>50</v>
@@ -691,10 +714,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -731,17 +754,8 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>0</v>
-      </c>
       <c r="B14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14">
-        <v>20</v>
-      </c>
-      <c r="E14" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -760,7 +774,7 @@
         <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C16">
         <v>20</v>
@@ -771,7 +785,7 @@
         <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C17">
         <v>12</v>
@@ -779,10 +793,10 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C18">
         <v>20</v>
@@ -790,7 +804,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -801,175 +815,191 @@
     </row>
     <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -979,6 +1009,6 @@
     <mergeCell ref="A20:G20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>